<commit_message>
Add TRANS OUTPT MATX in .xls
</commit_message>
<xml_diff>
--- a/TRANS_MATX_OUTPT_MATX.xlsx
+++ b/TRANS_MATX_OUTPT_MATX.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kpass\OneDrive\Рабочий стол\RPA\semestralka\Superstavy_Technologicka_Sekvence_Program\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5459597-65EF-42C2-8E41-A1F2A17B4CFD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="2145" yWindow="2880" windowWidth="18000" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -18,8 +24,52 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+  <si>
+    <t>TRANS MATX</t>
+  </si>
+  <si>
+    <t>A0</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>B0</t>
+  </si>
+  <si>
+    <t>B1</t>
+  </si>
+  <si>
+    <t>C0</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>Qt</t>
+  </si>
+  <si>
+    <t>OUTPT MATX</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>It</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -37,7 +87,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -45,12 +95,44 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +412,637 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="E4:M27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="E11" workbookViewId="0">
+      <selection activeCell="N27" sqref="N27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="F4" s="1"/>
+      <c r="G4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1">
+        <v>7</v>
+      </c>
+      <c r="G5" s="1">
+        <v>6</v>
+      </c>
+      <c r="H5" s="1">
+        <v>5</v>
+      </c>
+      <c r="I5" s="1">
+        <v>4</v>
+      </c>
+      <c r="J5" s="1">
+        <v>3</v>
+      </c>
+      <c r="K5" s="1">
+        <v>2</v>
+      </c>
+      <c r="L5" s="1">
+        <v>1</v>
+      </c>
+      <c r="M5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E6" s="3">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E7" s="3">
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E8" s="3">
+        <v>3</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E9" s="3">
+        <v>4</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>1</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E10" s="3">
+        <v>5</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
+      <c r="L10">
+        <v>1</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E11" s="3">
+        <v>6</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11">
+        <v>1</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E12" s="3">
+        <v>7</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <v>1</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>1</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E13" s="3">
+        <v>8</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
+      <c r="J13">
+        <v>1</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>1</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E14" s="3">
+        <v>9</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>1</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>1</v>
+      </c>
+      <c r="L14">
+        <v>1</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="J17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E18" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" s="1">
+        <v>7</v>
+      </c>
+      <c r="G18" s="1">
+        <v>6</v>
+      </c>
+      <c r="H18" s="1">
+        <v>5</v>
+      </c>
+      <c r="I18" s="1">
+        <v>4</v>
+      </c>
+      <c r="J18" s="1">
+        <v>3</v>
+      </c>
+      <c r="K18" s="1">
+        <v>2</v>
+      </c>
+      <c r="L18" s="1">
+        <v>1</v>
+      </c>
+      <c r="M18" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E19" s="3">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>1</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E20" s="3">
+        <v>2</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>1</v>
+      </c>
+      <c r="L20">
+        <v>1</v>
+      </c>
+      <c r="M20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E21" s="3">
+        <v>3</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>1</v>
+      </c>
+      <c r="K21">
+        <v>1</v>
+      </c>
+      <c r="L21">
+        <v>1</v>
+      </c>
+      <c r="M21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E22" s="3">
+        <v>4</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+      <c r="K22">
+        <v>1</v>
+      </c>
+      <c r="L22">
+        <v>0</v>
+      </c>
+      <c r="M22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E23" s="3">
+        <v>5</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E24" s="3">
+        <v>6</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <v>1</v>
+      </c>
+      <c r="M24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E25" s="3">
+        <v>7</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <v>1</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+      <c r="L25">
+        <v>1</v>
+      </c>
+      <c r="M25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E26" s="3">
+        <v>8</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <v>0</v>
+      </c>
+      <c r="K26">
+        <v>0</v>
+      </c>
+      <c r="L26">
+        <v>0</v>
+      </c>
+      <c r="M26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E27" s="3">
+        <v>9</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <v>1</v>
+      </c>
+      <c r="L27">
+        <v>0</v>
+      </c>
+      <c r="M27">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>